<commit_message>
Atualização automática de TUCUNDUVA.xlsx
</commit_message>
<xml_diff>
--- a/TUCUNDUVA.xlsx
+++ b/TUCUNDUVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15C3503D-519B-42C4-B46E-6B78B21BEE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EB98D19-9808-4A20-BBFA-C0297F2506C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,7 +1219,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{0CF1B122-F9DF-4091-92AC-C1744F124170}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4C169EC9-EDD8-433B-B502-B0F7F5D1EA68}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1249,10 +1249,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97799AED-A6D8-4474-BC7D-FE62D726C18F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3D5707-A181-4DD7-B966-34697675E0EF}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1290,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688AD505-1A4C-4B4D-861E-AD927358C9C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2403165A-61B9-4008-96F0-FC111CE32C16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1353,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B1B6A1F-071F-4A30-86C7-6069208320FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A161E893-4209-4521-96AB-9976653F1CB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1372,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5AF6803-8979-2C68-9CA6-065E798E906F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD071F0-27DE-4C55-FDBF-51AC206D276B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1421,7 +1421,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C7CBC2E-9AB2-3BE5-EB63-D2DCDA22E6E6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6ACA65-DB4C-9D15-4337-6E6A2F1F9491}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1440,7 +1440,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C54C36A8-6734-0743-480D-3777036C943E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC0167A9-1966-FFDB-143A-5C7FDF6EC143}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91D446CE-BE86-E868-FBB7-57A7F81E6A7C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8BCA61B-69A5-19BC-F431-D89D1FD18779}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1502,7 +1502,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B0E95E-838D-7E78-A818-DEA785E6BCCE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A252A543-3673-9D0A-E477-C54E4278021C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1545,7 +1545,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8B6F50-B52C-4593-9A23-2E823288AA40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{075089A6-1816-4579-A60A-932DAC6F5CE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1583,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2E4C016-B306-4E48-8B4A-9A4EC54CA777}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C768E4-C94A-4404-9D50-1F41A9E75199}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1626,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{414BBF98-2236-4D87-8D2E-FE7BD220AE7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B90FEE-59FC-40ED-8F2A-B682347AAB93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1939,7 +1939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BD2089-4051-44EE-9D1A-06A4F63FE551}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A728BA-4FBF-4F74-AC8A-5B9AEE85E067}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>